<commit_message>
Adding 3seg delay between requests.  Data removed from repository.
</commit_message>
<xml_diff>
--- a/data/results.xlsx
+++ b/data/results.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C85"/>
+  <dimension ref="A1:C103"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -415,131 +415,131 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>653019768585</v>
+        <v>276205836927</v>
       </c>
       <c r="B2" t="str">
-        <v>228458697</v>
+        <v>854636857</v>
       </c>
       <c r="C2" t="str">
-        <v>PENDING - UNABLE TO PROCESS REQUEST</v>
+        <v>DENIED - 1048 CUSTOMER NOT ELIGIBLE FOR MBG</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>776759943447</v>
+        <v>276205837018</v>
       </c>
       <c r="B3" t="str">
-        <v>853150250</v>
+        <v>854636857</v>
       </c>
       <c r="C3" t="str">
-        <v>DENIED - OT ON-TIME DELIVERY</v>
+        <v>DENIED - 1048 CUSTOMER NOT ELIGIBLE FOR MBG</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>776759943860</v>
+        <v>276205837040</v>
       </c>
       <c r="B4" t="str">
-        <v>853150250</v>
+        <v>854636857</v>
       </c>
       <c r="C4" t="str">
-        <v>DENIED - OT ON-TIME DELIVERY</v>
+        <v>PENDING - UNABLE TO PROCESS REQUEST (THANK YOU)</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>776759944053</v>
+        <v>276205837110</v>
       </c>
       <c r="B5" t="str">
-        <v>853150250</v>
+        <v>854636857</v>
       </c>
       <c r="C5" t="str">
-        <v>DENIED - OT ON-TIME DELIVERY</v>
+        <v>DENIED - 1048 CUSTOMER NOT ELIGIBLE FOR MBG</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>776759944579</v>
+        <v>276205837280</v>
       </c>
       <c r="B6" t="str">
-        <v>853150250</v>
+        <v>854636857</v>
       </c>
       <c r="C6" t="str">
-        <v>DENIED - OT ON-TIME DELIVERY</v>
+        <v>DENIED - 1048 CUSTOMER NOT ELIGIBLE FOR MBG</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>776759944638</v>
+        <v>276205837290</v>
       </c>
       <c r="B7" t="str">
-        <v>853150250</v>
+        <v>854636857</v>
       </c>
       <c r="C7" t="str">
-        <v>DENIED - OT ON-TIME DELIVERY</v>
+        <v>undefined</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>776759944796</v>
+        <v>276205837350</v>
       </c>
       <c r="B8" t="str">
-        <v>853150250</v>
+        <v>854636857</v>
       </c>
       <c r="C8" t="str">
-        <v>DENIED - OT ON-TIME DELIVERY</v>
+        <v>undefined</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>776759945027</v>
+        <v>276205838128</v>
       </c>
       <c r="B9" t="str">
-        <v>853150250</v>
+        <v>854636857</v>
       </c>
       <c r="C9" t="str">
-        <v>DENIED - OT ON-TIME DELIVERY</v>
+        <v>DENIED - 1048 CUSTOMER NOT ELIGIBLE FOR MBG</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>776759945185</v>
+        <v>276205838275</v>
       </c>
       <c r="B10" t="str">
-        <v>853150250</v>
+        <v>854636857</v>
       </c>
       <c r="C10" t="str">
-        <v>DENIED - OT ON-TIME DELIVERY</v>
+        <v>DENIED - 1048 CUSTOMER NOT ELIGIBLE FOR MBG</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>776759945862</v>
+        <v>276210463723</v>
       </c>
       <c r="B11" t="str">
-        <v>853150250</v>
+        <v>854636857</v>
       </c>
       <c r="C11" t="str">
-        <v>DENIED - OT ON-TIME DELIVERY</v>
+        <v>undefined</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>776759945965</v>
+        <v>276210464260</v>
       </c>
       <c r="B12" t="str">
-        <v>853150250</v>
+        <v>854636857</v>
       </c>
       <c r="C12" t="str">
-        <v>DENIED - OT ON-TIME DELIVERY</v>
+        <v>DENIED - 1048 CUSTOMER NOT ELIGIBLE FOR MBG</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>776759945987</v>
+        <v>276210465016</v>
       </c>
       <c r="B13" t="str">
-        <v>853150250</v>
+        <v>854636857</v>
       </c>
       <c r="C13" t="str">
         <v>PENDING - UNABLE TO PROCESS REQUEST (THANK YOU)</v>
@@ -547,549 +547,549 @@
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>776760001829</v>
+        <v>276211001856</v>
       </c>
       <c r="B14" t="str">
-        <v>853150250</v>
+        <v>854636857</v>
       </c>
       <c r="C14" t="str">
-        <v>DENIED - OT ON-TIME DELIVERY</v>
+        <v>DENIED - 1048 CUSTOMER NOT ELIGIBLE FOR MBG</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>776760001900</v>
+        <v>276211002326</v>
       </c>
       <c r="B15" t="str">
-        <v>853150250</v>
+        <v>854636857</v>
       </c>
       <c r="C15" t="str">
-        <v>DENIED - OT ON-TIME DELIVERY</v>
+        <v>Page didn't load.</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>776760002056</v>
+        <v>712336156030</v>
       </c>
       <c r="B16" t="str">
-        <v>853150250</v>
+        <v>854636857</v>
       </c>
       <c r="C16" t="str">
-        <v>DENIED - OT ON-TIME DELIVERY</v>
+        <v>PENDING - UNABLE TO PROCESS REQUEST (THANK YOU)</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>776760002160</v>
+        <v>712336156041</v>
       </c>
       <c r="B17" t="str">
-        <v>853150250</v>
+        <v>854636857</v>
       </c>
       <c r="C17" t="str">
-        <v>DENIED - OT ON-TIME DELIVERY</v>
+        <v>PENDING - UNABLE TO PROCESS REQUEST (THANK YOU)</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>776760002230</v>
+        <v>712336156052</v>
       </c>
       <c r="B18" t="str">
-        <v>853150250</v>
+        <v>854636857</v>
       </c>
       <c r="C18" t="str">
-        <v>PENDING - UNABLE TO PROCESS REQUEST (THANK YOU)</v>
+        <v>DENIED - 1048 CUSTOMER NOT ELIGIBLE FOR MBG</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>776760002505</v>
+        <v>712336156063</v>
       </c>
       <c r="B19" t="str">
-        <v>853150250</v>
+        <v>854636857</v>
       </c>
       <c r="C19" t="str">
-        <v>DENIED - OT ON-TIME DELIVERY</v>
+        <v>DENIED - 1048 CUSTOMER NOT ELIGIBLE FOR MBG</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>776760002527</v>
+        <v>712336156074</v>
       </c>
       <c r="B20" t="str">
-        <v>853150250</v>
+        <v>854636857</v>
       </c>
       <c r="C20" t="str">
-        <v>DENIED - OT ON-TIME DELIVERY</v>
+        <v>DENIED - 1048 CUSTOMER NOT ELIGIBLE FOR MBG</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>776760002733</v>
+        <v>712336156085</v>
       </c>
       <c r="B21" t="str">
-        <v>853150250</v>
+        <v>854636857</v>
       </c>
       <c r="C21" t="str">
-        <v>DENIED - OT ON-TIME DELIVERY</v>
+        <v>undefined</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>776760002961</v>
+        <v>712336156096</v>
       </c>
       <c r="B22" t="str">
-        <v>853150250</v>
+        <v>854636857</v>
       </c>
       <c r="C22" t="str">
-        <v>DENIED - OT ON-TIME DELIVERY</v>
+        <v>DENIED - 1048 CUSTOMER NOT ELIGIBLE FOR MBG</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>776760003155</v>
+        <v>712336156100</v>
       </c>
       <c r="B23" t="str">
-        <v>853150250</v>
+        <v>854636857</v>
       </c>
       <c r="C23" t="str">
-        <v>DENIED - OT ON-TIME DELIVERY</v>
+        <v>PENDING - UNABLE TO PROCESS REQUEST (THANK YOU)</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>776760003486</v>
+        <v>712336156111</v>
       </c>
       <c r="B24" t="str">
-        <v>853150250</v>
+        <v>854636857</v>
       </c>
       <c r="C24" t="str">
-        <v>DENIED - OT ON-TIME DELIVERY</v>
+        <v>PENDING - UNABLE TO PROCESS REQUEST (THANK YOU)</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>776760003681</v>
+        <v>712336156122</v>
       </c>
       <c r="B25" t="str">
-        <v>853150250</v>
+        <v>854636857</v>
       </c>
       <c r="C25" t="str">
-        <v>DENIED - OT ON-TIME DELIVERY</v>
+        <v>DENIED - 1048 CUSTOMER NOT ELIGIBLE FOR MBG</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>776760004335</v>
+        <v>712336156133</v>
       </c>
       <c r="B26" t="str">
-        <v>853150250</v>
+        <v>854636857</v>
       </c>
       <c r="C26" t="str">
-        <v>DENIED - OT ON-TIME DELIVERY</v>
+        <v>DENIED - 1048 CUSTOMER NOT ELIGIBLE FOR MBG</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>776760004460</v>
+        <v>712336156144</v>
       </c>
       <c r="B27" t="str">
-        <v>853150250</v>
+        <v>854636857</v>
       </c>
       <c r="C27" t="str">
-        <v>DENIED - OT ON-TIME DELIVERY</v>
+        <v>DENIED - 1048 CUSTOMER NOT ELIGIBLE FOR MBG</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>776751516202</v>
+        <v>712336156155</v>
       </c>
       <c r="B28" t="str">
-        <v>853208630</v>
+        <v>854636857</v>
       </c>
       <c r="C28" t="str">
-        <v>DENIED - OT ON-TIME DELIVERY</v>
+        <v>DENIED - 1048 CUSTOMER NOT ELIGIBLE FOR MBG</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>776751619351</v>
+        <v>712336156166</v>
       </c>
       <c r="B29" t="str">
-        <v>853208630</v>
+        <v>854636857</v>
       </c>
       <c r="C29" t="str">
-        <v>DENIED - OT ON-TIME DELIVERY</v>
+        <v>undefined</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>776756560910</v>
+        <v>712336156177</v>
       </c>
       <c r="B30" t="str">
-        <v>853208630</v>
+        <v>854636857</v>
       </c>
       <c r="C30" t="str">
-        <v>DENIED - OT ON-TIME DELIVERY</v>
+        <v>DENIED - 1048 CUSTOMER NOT ELIGIBLE FOR MBG</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>776757755887</v>
+        <v>712336156188</v>
       </c>
       <c r="B31" t="str">
-        <v>853208630</v>
+        <v>854636857</v>
       </c>
       <c r="C31" t="str">
-        <v>DENIED - OT ON-TIME DELIVERY</v>
+        <v>DENIED - 1048 CUSTOMER NOT ELIGIBLE FOR MBG</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>776759626089</v>
+        <v>712336156199</v>
       </c>
       <c r="B32" t="str">
-        <v>853208630</v>
+        <v>854636857</v>
       </c>
       <c r="C32" t="str">
-        <v>DENIED - OT ON-TIME DELIVERY</v>
+        <v>PENDING - UNABLE TO PROCESS REQUEST (THANK YOU)</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>776759626630</v>
+        <v>712336156203</v>
       </c>
       <c r="B33" t="str">
-        <v>853208630</v>
+        <v>854636857</v>
       </c>
       <c r="C33" t="str">
-        <v>DENIED - OT ON-TIME DELIVERY</v>
+        <v>DENIED - 1048 CUSTOMER NOT ELIGIBLE FOR MBG</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>776760372495</v>
+        <v>712336156214</v>
       </c>
       <c r="B34" t="str">
-        <v>853208630</v>
+        <v>854636857</v>
       </c>
       <c r="C34" t="str">
-        <v>DENIED - OT ON-TIME DELIVERY</v>
+        <v>Page didn't load.</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>776760478544</v>
+        <v>712336156225</v>
       </c>
       <c r="B35" t="str">
-        <v>853208630</v>
+        <v>854636857</v>
       </c>
       <c r="C35" t="str">
-        <v>DENIED - OT ON-TIME DELIVERY</v>
+        <v>Page didn't load.</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>776760575272</v>
+        <v>712336156236</v>
       </c>
       <c r="B36" t="str">
-        <v>853208630</v>
+        <v>854636857</v>
       </c>
       <c r="C36" t="str">
-        <v>DENIED - OT ON-TIME DELIVERY</v>
+        <v>Page didn't load.</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>776760694020</v>
+        <v>712336156247</v>
       </c>
       <c r="B37" t="str">
-        <v>853208630</v>
+        <v>854636857</v>
       </c>
       <c r="C37" t="str">
-        <v>DENIED - OT ON-TIME DELIVERY</v>
+        <v>Page didn't load.</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>776745049503</v>
+        <v>712336156258</v>
       </c>
       <c r="B38" t="str">
-        <v>853237539</v>
+        <v>854636857</v>
       </c>
       <c r="C38" t="str">
-        <v>DENIED - OT ON-TIME DELIVERY</v>
+        <v>Page didn't load.</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>776736764390</v>
+        <v>712336156269</v>
       </c>
       <c r="B39" t="str">
-        <v>853246715</v>
+        <v>854636857</v>
       </c>
       <c r="C39" t="str">
-        <v>APPROVED</v>
+        <v>Page didn't load.</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>776755430805</v>
+        <v>712336156270</v>
       </c>
       <c r="B40" t="str">
-        <v>853295997</v>
+        <v>854636857</v>
       </c>
       <c r="C40" t="str">
-        <v>DENIED - OT ON-TIME DELIVERY</v>
+        <v>Page didn't load.</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>776760126950</v>
+        <v>712336156280</v>
       </c>
       <c r="B41" t="str">
-        <v>853296119</v>
+        <v>854636857</v>
       </c>
       <c r="C41" t="str">
-        <v>DENIED - OT ON-TIME DELIVERY</v>
+        <v>Page didn't load.</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>776760386734</v>
+        <v>712336156291</v>
       </c>
       <c r="B42" t="str">
-        <v>853296119</v>
+        <v>854636857</v>
       </c>
       <c r="C42" t="str">
-        <v>DENIED - OT ON-TIME DELIVERY</v>
+        <v>Page didn't load.</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>776748200437</v>
+        <v>712336156306</v>
       </c>
       <c r="B43" t="str">
-        <v>228356472</v>
+        <v>854636857</v>
       </c>
       <c r="C43" t="str">
-        <v>DENIED - OT ON-TIME DELIVERY</v>
+        <v>Page didn't load.</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>776760990295</v>
+        <v>712336156317</v>
       </c>
       <c r="B44" t="str">
-        <v>853150250</v>
+        <v>854636857</v>
       </c>
       <c r="C44" t="str">
-        <v>DENIED - OT ON-TIME DELIVERY</v>
+        <v>Page didn't load.</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>776761514325</v>
+        <v>712336156328</v>
       </c>
       <c r="B45" t="str">
-        <v>853150250</v>
+        <v>854636857</v>
       </c>
       <c r="C45" t="str">
-        <v>DENIED - OT ON-TIME DELIVERY</v>
+        <v>Page didn't load.</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>776754087380</v>
+        <v>276286473902</v>
       </c>
       <c r="B46" t="str">
-        <v>853192839</v>
+        <v>854636857</v>
       </c>
       <c r="C46" t="str">
-        <v>DENIED - OT ON-TIME DELIVERY</v>
+        <v>Page didn't load.</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>776753793600</v>
+        <v>276384935515</v>
       </c>
       <c r="B47" t="str">
-        <v>853195352</v>
+        <v>854632136</v>
       </c>
       <c r="C47" t="str">
-        <v>DENIED - OT ON-TIME DELIVERY</v>
+        <v>Page didn't load.</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>776753793724</v>
+        <v>276395736903</v>
       </c>
       <c r="B48" t="str">
-        <v>853195352</v>
+        <v>854636857</v>
       </c>
       <c r="C48" t="str">
-        <v>DENIED - OT ON-TIME DELIVERY</v>
+        <v>Page didn't load.</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>776753794867</v>
+        <v>776934799067</v>
       </c>
       <c r="B49" t="str">
-        <v>853195352</v>
+        <v>228746251</v>
       </c>
       <c r="C49" t="str">
-        <v>DENIED - OT ON-TIME DELIVERY</v>
+        <v>Page didn't load.</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>776753795175</v>
+        <v>741573137145</v>
       </c>
       <c r="B50" t="str">
-        <v>853195352</v>
+        <v>855098238</v>
       </c>
       <c r="C50" t="str">
-        <v>DENIED - OT ON-TIME DELIVERY</v>
+        <v>Page didn't load.</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>776753795430</v>
+        <v>741573147628</v>
       </c>
       <c r="B51" t="str">
-        <v>853195352</v>
+        <v>855098238</v>
       </c>
       <c r="C51" t="str">
-        <v>DENIED - OT ON-TIME DELIVERY</v>
+        <v>Page didn't load.</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>776753795635</v>
+        <v>741573185445</v>
       </c>
       <c r="B52" t="str">
-        <v>853195352</v>
+        <v>855098238</v>
       </c>
       <c r="C52" t="str">
-        <v>DENIED - OT ON-TIME DELIVERY</v>
+        <v>Page didn't load.</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>776753795680</v>
+        <v>796788902170</v>
       </c>
       <c r="B53" t="str">
-        <v>853195352</v>
+        <v>855208497</v>
       </c>
       <c r="C53" t="str">
-        <v>DENIED - OT ON-TIME DELIVERY</v>
+        <v>Page didn't load.</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>776753795885</v>
+        <v>732596087956</v>
       </c>
       <c r="B54" t="str">
-        <v>853195352</v>
+        <v>855098238</v>
       </c>
       <c r="C54" t="str">
-        <v>DENIED - OT ON-TIME DELIVERY</v>
+        <v>Page didn't load.</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>776753796447</v>
+        <v>741573193101</v>
       </c>
       <c r="B55" t="str">
-        <v>853195352</v>
+        <v>855098238</v>
       </c>
       <c r="C55" t="str">
-        <v>PENDING - UNABLE TO PROCESS REQUEST (THANK YOU)</v>
+        <v>Page didn't load.</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>776753796701</v>
+        <v>651094080112</v>
       </c>
       <c r="B56" t="str">
-        <v>853195352</v>
+        <v>855098238</v>
       </c>
       <c r="C56" t="str">
-        <v>DENIED - OT ON-TIME DELIVERY</v>
+        <v>Page didn't load.</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v>776753796712</v>
+        <v>710000697981</v>
       </c>
       <c r="B57" t="str">
-        <v>853195352</v>
+        <v>855098238</v>
       </c>
       <c r="C57" t="str">
-        <v>DENIED - OT ON-TIME DELIVERY</v>
+        <v>Page didn't load.</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>776753797190</v>
+        <v>732596137233</v>
       </c>
       <c r="B58" t="str">
-        <v>853195352</v>
+        <v>855098238</v>
       </c>
       <c r="C58" t="str">
-        <v>DENIED - OT ON-TIME DELIVERY</v>
+        <v>Page didn't load.</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="str">
-        <v>776753797260</v>
+        <v>741573127486</v>
       </c>
       <c r="B59" t="str">
-        <v>853195352</v>
+        <v>855098238</v>
       </c>
       <c r="C59" t="str">
-        <v>DENIED - OT ON-TIME DELIVERY</v>
+        <v>Page didn't load.</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="str">
-        <v>776753797465</v>
+        <v>741573129673</v>
       </c>
       <c r="B60" t="str">
-        <v>853195352</v>
+        <v>855098238</v>
       </c>
       <c r="C60" t="str">
-        <v>DENIED - OT ON-TIME DELIVERY</v>
+        <v>Page didn't load.</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="str">
-        <v>776790956568</v>
+        <v>741573138829</v>
       </c>
       <c r="B61" t="str">
-        <v>853195352</v>
+        <v>855098238</v>
       </c>
       <c r="C61" t="str">
-        <v>APPROVED</v>
+        <v>Page didn't load.</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="str">
-        <v>776790956590</v>
+        <v>741573138830</v>
       </c>
       <c r="B62" t="str">
-        <v>853195352</v>
+        <v>855098238</v>
       </c>
       <c r="C62" t="str">
-        <v>APPROVED</v>
+        <v>Page didn't load.</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="str">
-        <v>776790956693</v>
+        <v>741573138900</v>
       </c>
       <c r="B63" t="str">
-        <v>853195352</v>
+        <v>855098238</v>
       </c>
       <c r="C63" t="str">
         <v>Page didn't load.</v>
@@ -1097,54 +1097,54 @@
     </row>
     <row r="64">
       <c r="A64" t="str">
-        <v>776790956888</v>
+        <v>741573140428</v>
       </c>
       <c r="B64" t="str">
-        <v>853195352</v>
+        <v>855098238</v>
       </c>
       <c r="C64" t="str">
-        <v>APPROVED</v>
+        <v>Page didn't load.</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="str">
-        <v>776790956903</v>
+        <v>741573158901</v>
       </c>
       <c r="B65" t="str">
-        <v>853195352</v>
+        <v>855098238</v>
       </c>
       <c r="C65" t="str">
-        <v>APPROVED</v>
+        <v>Page didn't load.</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="str">
-        <v>776790957299</v>
+        <v>741573166873</v>
       </c>
       <c r="B66" t="str">
-        <v>853195352</v>
+        <v>855098238</v>
       </c>
       <c r="C66" t="str">
-        <v>PENDING - UNABLE TO PROCESS REQUEST (THANK YOU)</v>
+        <v>Page didn't load.</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="str">
-        <v>776790957597</v>
+        <v>741573171725</v>
       </c>
       <c r="B67" t="str">
-        <v>853195352</v>
+        <v>855098238</v>
       </c>
       <c r="C67" t="str">
-        <v>APPROVED</v>
+        <v>Page didn't load.</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="str">
-        <v>776790958104</v>
+        <v>741573172560</v>
       </c>
       <c r="B68" t="str">
-        <v>853195352</v>
+        <v>855098238</v>
       </c>
       <c r="C68" t="str">
         <v>Page didn't load.</v>
@@ -1152,10 +1152,10 @@
     </row>
     <row r="69">
       <c r="A69" t="str">
-        <v>776790958376</v>
+        <v>741573191186</v>
       </c>
       <c r="B69" t="str">
-        <v>853195352</v>
+        <v>855098238</v>
       </c>
       <c r="C69" t="str">
         <v>Page didn't load.</v>
@@ -1163,10 +1163,10 @@
     </row>
     <row r="70">
       <c r="A70" t="str">
-        <v>776790958608</v>
+        <v>741573206859</v>
       </c>
       <c r="B70" t="str">
-        <v>853195352</v>
+        <v>855098238</v>
       </c>
       <c r="C70" t="str">
         <v>Page didn't load.</v>
@@ -1174,10 +1174,10 @@
     </row>
     <row r="71">
       <c r="A71" t="str">
-        <v>776790958972</v>
+        <v>276468889519</v>
       </c>
       <c r="B71" t="str">
-        <v>853195352</v>
+        <v>855098238</v>
       </c>
       <c r="C71" t="str">
         <v>Page didn't load.</v>
@@ -1185,10 +1185,10 @@
     </row>
     <row r="72">
       <c r="A72" t="str">
-        <v>776790959020</v>
+        <v>276468973659</v>
       </c>
       <c r="B72" t="str">
-        <v>853195352</v>
+        <v>855098238</v>
       </c>
       <c r="C72" t="str">
         <v>Page didn't load.</v>
@@ -1196,10 +1196,10 @@
     </row>
     <row r="73">
       <c r="A73" t="str">
-        <v>776790959214</v>
+        <v>741573137580</v>
       </c>
       <c r="B73" t="str">
-        <v>853195352</v>
+        <v>855098238</v>
       </c>
       <c r="C73" t="str">
         <v>Page didn't load.</v>
@@ -1207,10 +1207,10 @@
     </row>
     <row r="74">
       <c r="A74" t="str">
-        <v>776790959523</v>
+        <v>741573204282</v>
       </c>
       <c r="B74" t="str">
-        <v>853195352</v>
+        <v>855098238</v>
       </c>
       <c r="C74" t="str">
         <v>Page didn't load.</v>
@@ -1218,10 +1218,10 @@
     </row>
     <row r="75">
       <c r="A75" t="str">
-        <v>776790960354</v>
+        <v>741573206079</v>
       </c>
       <c r="B75" t="str">
-        <v>853195352</v>
+        <v>855098238</v>
       </c>
       <c r="C75" t="str">
         <v>Page didn't load.</v>
@@ -1229,10 +1229,10 @@
     </row>
     <row r="76">
       <c r="A76" t="str">
-        <v>776790960376</v>
+        <v>741573206080</v>
       </c>
       <c r="B76" t="str">
-        <v>853195352</v>
+        <v>855098238</v>
       </c>
       <c r="C76" t="str">
         <v>Page didn't load.</v>
@@ -1240,10 +1240,10 @@
     </row>
     <row r="77">
       <c r="A77" t="str">
-        <v>776790960961</v>
+        <v>741573206105</v>
       </c>
       <c r="B77" t="str">
-        <v>853195352</v>
+        <v>855098238</v>
       </c>
       <c r="C77" t="str">
         <v>Page didn't load.</v>
@@ -1251,10 +1251,10 @@
     </row>
     <row r="78">
       <c r="A78" t="str">
-        <v>776790961589</v>
+        <v>741573206116</v>
       </c>
       <c r="B78" t="str">
-        <v>853195352</v>
+        <v>855098238</v>
       </c>
       <c r="C78" t="str">
         <v>Page didn't load.</v>
@@ -1262,10 +1262,10 @@
     </row>
     <row r="79">
       <c r="A79" t="str">
-        <v>776790961898</v>
+        <v>741573206127</v>
       </c>
       <c r="B79" t="str">
-        <v>853195352</v>
+        <v>855098238</v>
       </c>
       <c r="C79" t="str">
         <v>Page didn't load.</v>
@@ -1273,10 +1273,10 @@
     </row>
     <row r="80">
       <c r="A80" t="str">
-        <v>713565891235</v>
+        <v>741573206230</v>
       </c>
       <c r="B80" t="str">
-        <v>853195415</v>
+        <v>855098238</v>
       </c>
       <c r="C80" t="str">
         <v>Page didn't load.</v>
@@ -1284,10 +1284,10 @@
     </row>
     <row r="81">
       <c r="A81" t="str">
-        <v>776742345139</v>
+        <v>741573206300</v>
       </c>
       <c r="B81" t="str">
-        <v>853246707</v>
+        <v>855098238</v>
       </c>
       <c r="C81" t="str">
         <v>Page didn't load.</v>
@@ -1295,10 +1295,10 @@
     </row>
     <row r="82">
       <c r="A82" t="str">
-        <v>776802392269</v>
+        <v>741573207145</v>
       </c>
       <c r="B82" t="str">
-        <v>228356459</v>
+        <v>855098238</v>
       </c>
       <c r="C82" t="str">
         <v>Page didn't load.</v>
@@ -1306,10 +1306,10 @@
     </row>
     <row r="83">
       <c r="A83" t="str">
-        <v>643408528019</v>
+        <v>741573207513</v>
       </c>
       <c r="B83" t="str">
-        <v>228356471</v>
+        <v>855098238</v>
       </c>
       <c r="C83" t="str">
         <v>Page didn't load.</v>
@@ -1317,10 +1317,10 @@
     </row>
     <row r="84">
       <c r="A84" t="str">
-        <v>275919110169</v>
+        <v>777072292750</v>
       </c>
       <c r="B84" t="str">
-        <v>228458935</v>
+        <v>855098238</v>
       </c>
       <c r="C84" t="str">
         <v>Page didn't load.</v>
@@ -1328,18 +1328,216 @@
     </row>
     <row r="85">
       <c r="A85" t="str">
-        <v>776831226776</v>
+        <v>777105256286</v>
       </c>
       <c r="B85" t="str">
-        <v>853195352</v>
+        <v>855098238</v>
       </c>
       <c r="C85" t="str">
+        <v>Page didn't load.</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="str">
+        <v>796577838900</v>
+      </c>
+      <c r="B86" t="str">
+        <v>855098238</v>
+      </c>
+      <c r="C86" t="str">
+        <v>Page didn't load.</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="str">
+        <v>796743355767</v>
+      </c>
+      <c r="B87" t="str">
+        <v>855098238</v>
+      </c>
+      <c r="C87" t="str">
+        <v>Page didn't load.</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="str">
+        <v>735869996455</v>
+      </c>
+      <c r="B88" t="str">
+        <v>855208497</v>
+      </c>
+      <c r="C88" t="str">
+        <v>Page didn't load.</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="str">
+        <v>735869996466</v>
+      </c>
+      <c r="B89" t="str">
+        <v>855208497</v>
+      </c>
+      <c r="C89" t="str">
+        <v>Page didn't load.</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="str">
+        <v>735869996477</v>
+      </c>
+      <c r="B90" t="str">
+        <v>855208497</v>
+      </c>
+      <c r="C90" t="str">
+        <v>Page didn't load.</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="str">
+        <v>735869996499</v>
+      </c>
+      <c r="B91" t="str">
+        <v>855208497</v>
+      </c>
+      <c r="C91" t="str">
+        <v>Page didn't load.</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="str">
+        <v>735869996503</v>
+      </c>
+      <c r="B92" t="str">
+        <v>855208497</v>
+      </c>
+      <c r="C92" t="str">
+        <v>Page didn't load.</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="str">
+        <v>796715308073</v>
+      </c>
+      <c r="B93" t="str">
+        <v>855208497</v>
+      </c>
+      <c r="C93" t="str">
+        <v>Page didn't load.</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="str">
+        <v>796788944165</v>
+      </c>
+      <c r="B94" t="str">
+        <v>855208497</v>
+      </c>
+      <c r="C94" t="str">
+        <v>Page didn't load.</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="str">
+        <v>796800222590</v>
+      </c>
+      <c r="B95" t="str">
+        <v>855208497</v>
+      </c>
+      <c r="C95" t="str">
+        <v>Page didn't load.</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="str">
+        <v>796814013265</v>
+      </c>
+      <c r="B96" t="str">
+        <v>855208497</v>
+      </c>
+      <c r="C96" t="str">
+        <v>Page didn't load.</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="str">
+        <v>796827271138</v>
+      </c>
+      <c r="B97" t="str">
+        <v>855208497</v>
+      </c>
+      <c r="C97" t="str">
+        <v>Page didn't load.</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="str">
+        <v>796827277700</v>
+      </c>
+      <c r="B98" t="str">
+        <v>855208497</v>
+      </c>
+      <c r="C98" t="str">
+        <v>Page didn't load.</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="str">
+        <v>796827285340</v>
+      </c>
+      <c r="B99" t="str">
+        <v>855208497</v>
+      </c>
+      <c r="C99" t="str">
+        <v>Page didn't load.</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="str">
+        <v>796827285410</v>
+      </c>
+      <c r="B100" t="str">
+        <v>855208497</v>
+      </c>
+      <c r="C100" t="str">
+        <v>Page didn't load.</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="str">
+        <v>0</v>
+      </c>
+      <c r="B101" t="str">
+        <v>0</v>
+      </c>
+      <c r="C101" t="str">
+        <v>Page didn't load.</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="str">
+        <v>0</v>
+      </c>
+      <c r="B102" t="str">
+        <v>0</v>
+      </c>
+      <c r="C102" t="str">
+        <v>Page didn't load.</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="str">
+        <v>0</v>
+      </c>
+      <c r="B103" t="str">
+        <v>0</v>
+      </c>
+      <c r="C103" t="str">
         <v>Page didn't load.</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C85"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C103"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>